<commit_message>
A fwe changes in field mappings and distributor lookup.
</commit_message>
<xml_diff>
--- a/distributorLookup.xlsx
+++ b/distributorLookup.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="201">
   <si>
     <t>Advanide</t>
   </si>
@@ -616,6 +616,18 @@
   </si>
   <si>
     <t>serial</t>
+  </si>
+  <si>
+    <t>WT Microelectronics</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>Ryoyo Semicon</t>
+  </si>
+  <si>
+    <t>ryoyo</t>
   </si>
 </sst>
 </file>
@@ -958,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ55"/>
+  <dimension ref="A1:AQ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,6 +1468,22 @@
       </c>
       <c r="B55" s="6" t="s">
         <v>196</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>